<commit_message>
BRICS et Proportion dans le temps
</commit_message>
<xml_diff>
--- a/BDD/Canada/energy-canada.xlsx
+++ b/BDD/Canada/energy-canada.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leatr\Documents\Césure\Zenon\EnergyLimits\BDD\Canada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{108EBFC2-8D95-4611-B7DE-35208F62756A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DA3D2A-0155-46F4-8CE0-77D6D7F6EF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1115C400-9D94-4DF6-B58A-0DF3FB51F98E}"/>
+    <workbookView minimized="1" xWindow="1152" yWindow="1044" windowWidth="11364" windowHeight="11916" xr2:uid="{1115C400-9D94-4DF6-B58A-0DF3FB51F98E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD8EACA-B152-4CCA-9D75-624E8344AF46}">
   <dimension ref="A1:B217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C45" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>

</xml_diff>